<commit_message>
Update errors and add pointer
</commit_message>
<xml_diff>
--- a/DatasetRichter_onboard.xlsx
+++ b/DatasetRichter_onboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/amr8004_psu_edu/Documents/ULTERA-Richter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xander\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{FD1939D1-6A67-7B41-BA20-173BA948657A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D26CBDA2-6F1C-423E-8394-82081DA586B7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66376896-8355-41F0-91FC-990830051588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20736" yWindow="-4248" windowWidth="20832" windowHeight="17376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
   <si>
     <t>Metadata</t>
   </si>
@@ -344,27 +344,18 @@
     <t>HCP</t>
   </si>
   <si>
-    <t>10.2320/matertrans.MT-M2019213</t>
-  </si>
-  <si>
     <t>MT-C</t>
   </si>
   <si>
     <t>Ir29.0678 Rh29.0678 Ru11.8644 W15 Mo15</t>
   </si>
   <si>
-    <t>10.2320/matertrans.MT-M2019214</t>
-  </si>
-  <si>
     <t>MT-D</t>
   </si>
   <si>
     <t>Ir34.8814 Rh34.8814 Ru14.2373 W8 Mo8</t>
   </si>
   <si>
-    <t>10.2320/matertrans.MT-M2019215</t>
-  </si>
-  <si>
     <t>MT-E</t>
   </si>
   <si>
@@ -374,13 +365,13 @@
     <t>FCC</t>
   </si>
   <si>
-    <t>10.2320/matertrans.MT-M2019216</t>
-  </si>
-  <si>
     <t>MT-Cprime</t>
   </si>
   <si>
     <t>annealed at 1273K for 200h</t>
+  </si>
+  <si>
+    <t>T2</t>
   </si>
 </sst>
 </file>
@@ -1062,6 +1053,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1111,33 +1129,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1423,28 +1414,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D15"/>
+    <sheetView tabSelected="1" topLeftCell="I8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="3" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="6" width="17.81640625" customWidth="1"/>
+    <col min="7" max="7" width="19.26953125" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1"/>
-    <col min="14" max="14" width="34.7109375" customWidth="1"/>
-    <col min="15" max="15" width="39.28515625" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" customWidth="1"/>
+    <col min="11" max="11" width="15.26953125" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" customWidth="1"/>
+    <col min="13" max="13" width="17.81640625" customWidth="1"/>
+    <col min="14" max="14" width="34.7265625" customWidth="1"/>
+    <col min="15" max="15" width="39.26953125" customWidth="1"/>
+    <col min="16" max="16" width="17.7265625" customWidth="1"/>
     <col min="17" max="18" width="18" customWidth="1"/>
-    <col min="19" max="20" width="17.42578125" customWidth="1"/>
+    <col min="19" max="20" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16.5" thickTop="1" thickBot="1">
@@ -1459,39 +1450,39 @@
       <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="43"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="52"/>
       <c r="O2" s="26"/>
     </row>
-    <row r="3" spans="1:20" ht="21.95" customHeight="1" thickBot="1">
+    <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="45"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="54"/>
       <c r="O3" s="26"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1">
@@ -1502,50 +1493,50 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="21.6" customHeight="1" thickBot="1">
+    <row r="5" spans="1:20" ht="21.65" customHeight="1" thickBot="1">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="66" t="s">
+      <c r="H5" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="59" t="s">
+      <c r="L5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="59" t="s">
+      <c r="M5" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="59" t="s">
+      <c r="N5" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="60" t="s">
+      <c r="O5" s="42" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1556,21 +1547,21 @@
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="61"/>
-    </row>
-    <row r="7" spans="1:20" ht="15.95" thickBot="1">
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="43"/>
+    </row>
+    <row r="7" spans="1:20" ht="16" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1613,7 +1604,7 @@
       <c r="N7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="62"/>
+      <c r="O7" s="44"/>
       <c r="P7" s="32" t="s">
         <v>36</v>
       </c>
@@ -1624,39 +1615,39 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="20.45" customHeight="1" thickTop="1" thickBot="1">
+    <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="53" t="s">
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="56" t="s">
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="57"/>
+      <c r="N8" s="66"/>
       <c r="O8" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="63" t="s">
+      <c r="P8" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="64"/>
-      <c r="R8" s="64"/>
-      <c r="S8" s="64"/>
-      <c r="T8" s="65"/>
-    </row>
-    <row r="9" spans="1:20" ht="21.95" customHeight="1" thickBot="1">
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="47"/>
+    </row>
+    <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1">
       <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
@@ -1739,7 +1730,9 @@
       <c r="J10" s="33"/>
       <c r="K10" s="33"/>
       <c r="L10" s="35"/>
-      <c r="M10" s="34"/>
+      <c r="M10" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="N10" s="20" t="s">
         <v>68</v>
       </c>
@@ -1768,18 +1761,20 @@
       <c r="J11" s="33"/>
       <c r="K11" s="33"/>
       <c r="L11" s="35"/>
-      <c r="M11" s="34"/>
+      <c r="M11" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="N11" s="20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="O11" s="20"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>74</v>
       </c>
       <c r="C12" s="34" t="s">
         <v>71</v>
@@ -1797,18 +1792,20 @@
       <c r="J12" s="33"/>
       <c r="K12" s="33"/>
       <c r="L12" s="35"/>
-      <c r="M12" s="34"/>
+      <c r="M12" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="N12" s="20" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="O12" s="21"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>71</v>
@@ -1826,21 +1823,23 @@
       <c r="J13" s="33"/>
       <c r="K13" s="33"/>
       <c r="L13" s="35"/>
-      <c r="M13" s="34"/>
+      <c r="M13" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="N13" s="20" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="O13" s="20"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D14" s="34" t="s">
         <v>66</v>
@@ -1855,18 +1854,20 @@
       <c r="J14" s="33"/>
       <c r="K14" s="33"/>
       <c r="L14" s="35"/>
-      <c r="M14" s="34"/>
+      <c r="M14" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="N14" s="20" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="O14" s="20"/>
     </row>
-    <row r="15" spans="1:20" ht="15">
+    <row r="15" spans="1:20">
       <c r="A15" s="20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="34" t="s">
         <v>71</v>
@@ -1875,7 +1876,7 @@
         <v>66</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="34"/>
@@ -1884,9 +1885,11 @@
       <c r="J15" s="33"/>
       <c r="K15" s="33"/>
       <c r="L15" s="35"/>
-      <c r="M15" s="34"/>
+      <c r="M15" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="N15" s="20" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="O15" s="21"/>
     </row>
@@ -8058,11 +8061,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -8077,6 +8075,11 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
property name & number errors fix
</commit_message>
<xml_diff>
--- a/DatasetRichter_onboard.xlsx
+++ b/DatasetRichter_onboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xander\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04913E6A-1B49-4FD7-B2CF-CAA048F2E7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87920B9E-3CFD-44E0-A771-9B8C4EA20408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20736" yWindow="-4248" windowWidth="20832" windowHeight="17376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="158">
   <si>
     <t>Metadata</t>
   </si>
@@ -527,24 +527,15 @@
     <t>msea-an</t>
   </si>
   <si>
-    <t>Nb24 Sc25 Ti25 Zr25</t>
-  </si>
-  <si>
     <t>AAM+A</t>
   </si>
   <si>
     <t>HCP+BCC</t>
   </si>
   <si>
-    <t>Nb24 Sc25 Ti25 Zr26</t>
-  </si>
-  <si>
     <t>HCP plate in BCC matrix</t>
   </si>
   <si>
-    <t>HCP plate in BCC matrix, annealed at 1000C for 24hr</t>
-  </si>
-  <si>
     <t>10.1016/j.jallcom.2016.01.153</t>
   </si>
   <si>
@@ -557,21 +548,9 @@
     <t>JAC-2</t>
   </si>
   <si>
-    <t>Co Cr Fe Ni Nb0.26</t>
-  </si>
-  <si>
-    <t>FCC+FCC</t>
-  </si>
-  <si>
     <t>hypoeutectic</t>
   </si>
   <si>
-    <t>FCC precipitates in hypoeutectic, 750C 7 days</t>
-  </si>
-  <si>
-    <t>ultimate compressive strain</t>
-  </si>
-  <si>
     <t>10.1016/j.jallcom.2015.09.153</t>
   </si>
   <si>
@@ -608,13 +587,19 @@
     <t>divorced eutectic</t>
   </si>
   <si>
-    <t>ultimate comporessive strain</t>
-  </si>
-  <si>
-    <t>minimum comporessive strain</t>
-  </si>
-  <si>
     <t>minimum compressive strength</t>
+  </si>
+  <si>
+    <t>Nb25 Sc25 Ti25 Zr25</t>
+  </si>
+  <si>
+    <t>FCC+laves+FCC</t>
+  </si>
+  <si>
+    <t>FCC precipitates in hypoeutectic; anneal at 750C for 7 days</t>
+  </si>
+  <si>
+    <t>HCP plate in BCC matrix; annealed at 1000C for 24hr</t>
   </si>
 </sst>
 </file>
@@ -1659,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N64" sqref="N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3559,16 +3544,16 @@
         <v>131</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D51" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F51" s="34" t="s">
         <v>121</v>
@@ -3598,16 +3583,16 @@
         <v>132</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C52" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D52" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E52" s="20" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="F52" s="34" t="s">
         <v>121</v>
@@ -3637,16 +3622,16 @@
         <v>131</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D53" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F53" s="34" t="s">
         <v>120</v>
@@ -3675,16 +3660,16 @@
         <v>132</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C54" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D54" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="F54" s="34" t="s">
         <v>120</v>
@@ -3713,16 +3698,16 @@
         <v>131</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="C55" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D55" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F55" s="34" t="s">
         <v>109</v>
@@ -3751,16 +3736,16 @@
         <v>132</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C56" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="F56" s="34" t="s">
         <v>109</v>
@@ -3789,19 +3774,19 @@
         <v>131</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="C57" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D57" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F57" s="34" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="G57" s="34" t="s">
         <v>29</v>
@@ -3827,19 +3812,19 @@
         <v>132</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C58" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D58" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="F58" s="34" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="G58" s="34" t="s">
         <v>29</v>
@@ -3849,7 +3834,7 @@
         <v>298</v>
       </c>
       <c r="J58" s="33">
-        <v>20</v>
+        <v>28.2</v>
       </c>
       <c r="K58" s="33"/>
       <c r="L58" s="20" t="s">
@@ -3862,19 +3847,19 @@
     </row>
     <row r="59" spans="1:17">
       <c r="A59" s="37" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C59" s="34" t="s">
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="D59" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E59" s="20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F59" s="34" t="s">
         <v>121</v>
@@ -3896,24 +3881,24 @@
       </c>
       <c r="M59" s="20"/>
       <c r="N59" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:17">
       <c r="A60" s="37" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C60" s="34" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="D60" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E60" s="20" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F60" s="34" t="s">
         <v>121</v>
@@ -3935,24 +3920,24 @@
       </c>
       <c r="M60" s="20"/>
       <c r="N60" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:17">
       <c r="A61" s="37" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C61" s="34" t="s">
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="D61" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E61" s="20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F61" s="34" t="s">
         <v>120</v>
@@ -3973,24 +3958,24 @@
       </c>
       <c r="M61" s="20"/>
       <c r="N61" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:17">
       <c r="A62" s="37" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C62" s="34" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="D62" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F62" s="34" t="s">
         <v>120</v>
@@ -4011,27 +3996,27 @@
       </c>
       <c r="M62" s="20"/>
       <c r="N62" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:17">
       <c r="A63" s="37" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C63" s="34" t="s">
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="D63" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F63" s="34" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="G63" s="34" t="s">
         <v>29</v>
@@ -4041,7 +4026,7 @@
         <v>298</v>
       </c>
       <c r="J63" s="33">
-        <v>325</v>
+        <v>40</v>
       </c>
       <c r="K63" s="33"/>
       <c r="L63" s="20" t="s">
@@ -4049,27 +4034,27 @@
       </c>
       <c r="M63" s="20"/>
       <c r="N63" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:17">
       <c r="A64" s="37" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C64" s="34" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D64" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F64" s="34" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="G64" s="34" t="s">
         <v>29</v>
@@ -4087,24 +4072,24 @@
       </c>
       <c r="M64" s="20"/>
       <c r="N64" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:14">
       <c r="A65" s="37" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C65" s="34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D65" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E65" s="20" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F65" s="34" t="s">
         <v>121</v>
@@ -4126,24 +4111,24 @@
       </c>
       <c r="M65" s="20"/>
       <c r="N65" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:14">
       <c r="A66" s="37" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B66" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" s="34" t="s">
         <v>150</v>
-      </c>
-      <c r="C66" s="34" t="s">
-        <v>157</v>
       </c>
       <c r="D66" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E66" s="20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F66" s="34" t="s">
         <v>121</v>
@@ -4165,24 +4150,24 @@
       </c>
       <c r="M66" s="20"/>
       <c r="N66" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:14">
       <c r="A67" s="37" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C67" s="34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D67" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E67" s="20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F67" s="34" t="s">
         <v>121</v>
@@ -4204,24 +4189,24 @@
       </c>
       <c r="M67" s="20"/>
       <c r="N67" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:14">
       <c r="A68" s="37" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C68" s="34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D68" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E68" s="20" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F68" s="34" t="s">
         <v>121</v>
@@ -4243,27 +4228,27 @@
       </c>
       <c r="M68" s="20"/>
       <c r="N68" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:14">
       <c r="A69" s="37" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C69" s="34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D69" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E69" s="20" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F69" s="34" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="G69" s="34" t="s">
         <v>29</v>
@@ -4281,24 +4266,24 @@
       </c>
       <c r="M69" s="20"/>
       <c r="N69" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:14">
       <c r="A70" s="37" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B70" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" s="34" t="s">
         <v>150</v>
-      </c>
-      <c r="C70" s="34" t="s">
-        <v>157</v>
       </c>
       <c r="D70" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E70" s="20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F70" s="34" t="s">
         <v>120</v>
@@ -4319,24 +4304,24 @@
       </c>
       <c r="M70" s="20"/>
       <c r="N70" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:14">
       <c r="A71" s="37" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C71" s="34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D71" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F71" s="34" t="s">
         <v>120</v>
@@ -4357,24 +4342,24 @@
       </c>
       <c r="M71" s="20"/>
       <c r="N71" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:14">
       <c r="A72" s="37" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C72" s="34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D72" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E72" s="20" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F72" s="34" t="s">
         <v>120</v>
@@ -4395,27 +4380,27 @@
       </c>
       <c r="M72" s="20"/>
       <c r="N72" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:14">
       <c r="A73" s="37" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B73" s="20" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C73" s="34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D73" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E73" s="20" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F73" s="34" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G73" s="34" t="s">
         <v>29</v>
@@ -4433,27 +4418,27 @@
       </c>
       <c r="M73" s="20"/>
       <c r="N73" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="37" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B74" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" s="34" t="s">
         <v>150</v>
-      </c>
-      <c r="C74" s="34" t="s">
-        <v>157</v>
       </c>
       <c r="D74" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F74" s="34" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="G74" s="34" t="s">
         <v>29</v>
@@ -4463,7 +4448,7 @@
         <v>298</v>
       </c>
       <c r="J74" s="33">
-        <v>38.5</v>
+        <v>40</v>
       </c>
       <c r="K74" s="33"/>
       <c r="L74" s="20" t="s">
@@ -4471,27 +4456,27 @@
       </c>
       <c r="M74" s="20"/>
       <c r="N74" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:14">
       <c r="A75" s="37" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B75" s="20" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C75" s="34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D75" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E75" s="20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F75" s="34" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="G75" s="34" t="s">
         <v>29</v>
@@ -4501,7 +4486,7 @@
         <v>298</v>
       </c>
       <c r="J75" s="33">
-        <v>23.5</v>
+        <v>25</v>
       </c>
       <c r="K75" s="33"/>
       <c r="L75" s="20" t="s">
@@ -4509,27 +4494,27 @@
       </c>
       <c r="M75" s="20"/>
       <c r="N75" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="37" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B76" s="20" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C76" s="34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D76" s="34" t="s">
         <v>107</v>
       </c>
       <c r="E76" s="20" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F76" s="34" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="G76" s="34" t="s">
         <v>29</v>
@@ -4539,7 +4524,7 @@
         <v>298</v>
       </c>
       <c r="J76" s="33">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="K76" s="33"/>
       <c r="L76" s="20" t="s">
@@ -4547,7 +4532,7 @@
       </c>
       <c r="M76" s="20"/>
       <c r="N76" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:14">

</xml_diff>